<commit_message>
Updated round 3 results + round 4 predictions
Updated round 3 results after all 26-06 matches were played
Added round 4 match result predictions
</commit_message>
<xml_diff>
--- a/Football match predictions/Statistics/Country statistics - After round 3.xlsx
+++ b/Football match predictions/Statistics/Country statistics - After round 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larsl\Documents\Privé\Data Analysis\Football-match-predictions\Football match predictions\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3E1761-EBD7-498E-A316-83B0CFE8973C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E86241-93E5-46CD-96CC-B660E5677B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="13" xr2:uid="{381A2E7C-6258-4120-A37E-4E40B62320C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="21" xr2:uid="{381A2E7C-6258-4120-A37E-4E40B62320C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Rankings" sheetId="25" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="230">
   <si>
     <t>Mexico</t>
   </si>
@@ -8137,7 +8137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59ED8576-7ACE-45FB-B056-6602C6070749}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
@@ -10593,10 +10593,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7411AC2-5D21-455D-BE63-80B3767F1FFF}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="O17" sqref="O17:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11513,6 +11513,60 @@
       <c r="P17">
         <f t="shared" ref="P17" si="4">AVERAGE(M12:M16)</f>
         <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18">
+        <f>_xlfn.XLOOKUP(F18,Rankings!B:B,Rankings!A:A)</f>
+        <v>48</v>
+      </c>
+      <c r="H18">
+        <f>_xlfn.XLOOKUP(F18, Rankings!B:B, Rankings!C:C)</f>
+        <v>1461.55</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18" si="5">AVERAGE(L13:L17)</f>
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18" si="6">AVERAGE(M13:M17)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -11525,10 +11579,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA8C81D-E431-43F0-97F0-FC4B37BE9C98}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16:P17"/>
+      <selection activeCell="O17" sqref="O17:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12444,6 +12498,60 @@
       </c>
       <c r="P17">
         <f t="shared" ref="P17" si="4">AVERAGE(M12:M16)</f>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18">
+        <f>_xlfn.XLOOKUP(F18,Rankings!B:B,Rankings!A:A)</f>
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <f>_xlfn.XLOOKUP(F18, Rankings!B:B, Rankings!C:C)</f>
+        <v>1795.23</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18" si="5">AVERAGE(L13:L17)</f>
+        <v>1.4</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18" si="6">AVERAGE(M13:M17)</f>
         <v>1.4</v>
       </c>
     </row>
@@ -12457,10 +12565,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC26FBD-B83A-45BD-ADA0-0A70FF1AAFE8}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="O20" sqref="O20:P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13538,6 +13646,60 @@
       </c>
       <c r="P20">
         <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <f>_xlfn.XLOOKUP(F21,Rankings!B:B,Rankings!A:A)</f>
+        <v>22</v>
+      </c>
+      <c r="H21">
+        <f>_xlfn.XLOOKUP(F21, Rankings!B:B, Rankings!C:C)</f>
+        <v>1568.86</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <f>AVERAGE(L16:L20)</f>
+        <v>1.8</v>
+      </c>
+      <c r="P21">
+        <f t="shared" ref="P21" si="3">AVERAGE(M16:M20)</f>
         <v>0.6</v>
       </c>
     </row>
@@ -13551,10 +13713,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5DCFAA-A4DC-4488-B50C-5FAD324B64FC}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="O17" sqref="O17:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14470,6 +14632,60 @@
       </c>
       <c r="P17">
         <f t="shared" ref="P17" si="4">AVERAGE(M12:M16)</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18">
+        <f>_xlfn.XLOOKUP(F18,Rankings!B:B,Rankings!A:A)</f>
+        <v>46</v>
+      </c>
+      <c r="H18">
+        <f>_xlfn.XLOOKUP(F18, Rankings!B:B, Rankings!C:C)</f>
+        <v>1468.17</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18" si="5">AVERAGE(L13:L17)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18" si="6">AVERAGE(M13:M17)</f>
         <v>0.6</v>
       </c>
     </row>
@@ -17930,10 +18146,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFDBCB3-D360-40C8-B08C-914750BA416F}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18850,6 +19066,60 @@
       <c r="P17">
         <f t="shared" ref="P17" si="4">AVERAGE(M12:M16)</f>
         <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18">
+        <f>_xlfn.XLOOKUP(F18,Rankings!B:B,Rankings!A:A)</f>
+        <v>36</v>
+      </c>
+      <c r="H18">
+        <f>_xlfn.XLOOKUP(F18, Rankings!B:B, Rankings!C:C)</f>
+        <v>1501.47</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18" si="5">AVERAGE(L13:L17)</f>
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18" si="6">AVERAGE(M13:M17)</f>
+        <v>2.4</v>
       </c>
     </row>
   </sheetData>
@@ -18862,10 +19132,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1666DE3-0108-4BD1-8BCD-C23A383A5ADE}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="O16" sqref="O16:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19728,6 +19998,60 @@
       <c r="P16">
         <f t="shared" ref="P16" si="4">AVERAGE(M11:M15)</f>
         <v>1.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17">
+        <f>_xlfn.XLOOKUP(F17,Rankings!B:B,Rankings!A:A)</f>
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <f>_xlfn.XLOOKUP(F17, Rankings!B:B, Rankings!C:C)</f>
+        <v>1748.11</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>6</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <f t="shared" ref="O17" si="5">AVERAGE(L12:L16)</f>
+        <v>1.4</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ref="P17" si="6">AVERAGE(M12:M16)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -19743,10 +20067,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74565D70-9BAA-4DFF-8CD4-0A8FCCB8554C}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20933,6 +21257,60 @@
       <c r="P22">
         <f t="shared" ref="P22" si="4">AVERAGE(M17:M21)</f>
         <v>1.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23">
+        <f>_xlfn.XLOOKUP(F23,Rankings!B:B,Rankings!A:A)</f>
+        <v>75</v>
+      </c>
+      <c r="H23">
+        <f>_xlfn.XLOOKUP(F23, Rankings!B:B, Rankings!C:C)</f>
+        <v>1333.76</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>2</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ref="O23" si="5">AVERAGE(L18:L22)</f>
+        <v>2.6</v>
+      </c>
+      <c r="P23">
+        <f t="shared" ref="P23" si="6">AVERAGE(M18:M22)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -20948,10 +21326,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC37B67-26A1-487C-8F6E-3E36DA5FFAF0}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21868,6 +22246,60 @@
       </c>
       <c r="P17">
         <f t="shared" ref="P17" si="4">AVERAGE(M12:M16)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18">
+        <f>_xlfn.XLOOKUP(F18,Rankings!B:B,Rankings!A:A)</f>
+        <v>40</v>
+      </c>
+      <c r="H18">
+        <f>_xlfn.XLOOKUP(F18, Rankings!B:B, Rankings!C:C)</f>
+        <v>1495.94</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18" si="5">AVERAGE(L13:L17)</f>
+        <v>2.6</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18" si="6">AVERAGE(M13:M17)</f>
         <v>1.2</v>
       </c>
     </row>

</xml_diff>